<commit_message>
First homework is updated
</commit_message>
<xml_diff>
--- a/2016-07-12/FIME-8A/Homework001/db/questions.xlsx
+++ b/2016-07-12/FIME-8A/Homework001/db/questions.xlsx
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="questions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1056,7 +1056,7 @@
   <dimension ref="A1:BB23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G23" sqref="G2:M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1235,6 +1235,50 @@
       <c r="B2" t="s">
         <v>54</v>
       </c>
+      <c r="C2">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="D2">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>4</v>
+      </c>
+      <c r="E2">
+        <f t="shared" ref="E2:M23" ca="1" si="0">RANDBETWEEN(2,9)</f>
+        <v>7</v>
+      </c>
+      <c r="F2">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G2">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H2">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K2">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M2">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -1243,6 +1287,50 @@
       <c r="B3" t="s">
         <v>55</v>
       </c>
+      <c r="C3">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="C3:D17" ca="1" si="1">RANDBETWEEN(2,9)</f>
+        <v>8</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -1251,6 +1339,50 @@
       <c r="B4" t="s">
         <v>56</v>
       </c>
+      <c r="C4">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>5</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -1259,6 +1391,50 @@
       <c r="B5" t="s">
         <v>57</v>
       </c>
+      <c r="C5">
+        <f ca="1">RANDBETWEEN(2,9)</f>
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="F5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G5">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M5">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1267,6 +1443,50 @@
       <c r="B6" t="s">
         <v>58</v>
       </c>
+      <c r="C6">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E6">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G6">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H6">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I6">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K6">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L6">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M6">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -1275,6 +1495,50 @@
       <c r="B7" t="s">
         <v>59</v>
       </c>
+      <c r="C7">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G7">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H7">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I7">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J7">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L7">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="8" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -1283,6 +1547,50 @@
       <c r="B8" t="s">
         <v>60</v>
       </c>
+      <c r="C8">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G8">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H8">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J8">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K8">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1291,6 +1599,50 @@
       <c r="B9" t="s">
         <v>61</v>
       </c>
+      <c r="C9">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ca="1" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="E9">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G9">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J9">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K9">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L9">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M9">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1299,6 +1651,50 @@
       <c r="B10" t="s">
         <v>62</v>
       </c>
+      <c r="C10">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E10">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="I10">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K10">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="M10">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="11" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1307,6 +1703,50 @@
       <c r="B11" t="s">
         <v>63</v>
       </c>
+      <c r="C11">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E11">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="G11">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H11">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J11">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K11">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1315,6 +1755,50 @@
       <c r="B12" t="s">
         <v>64</v>
       </c>
+      <c r="C12">
+        <f t="shared" ca="1" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G12">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="H12">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J12">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K12">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="L12">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M12">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="13" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1323,6 +1807,50 @@
       <c r="B13" t="s">
         <v>65</v>
       </c>
+      <c r="C13">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <f t="shared" ca="1" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="E13">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F13">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H13">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I13">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J13">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K13">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L13">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M13">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="14" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1331,6 +1859,50 @@
       <c r="B14" t="s">
         <v>66</v>
       </c>
+      <c r="C14">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ca="1" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="E14">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F14">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H14">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I14">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K14">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L14">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="M14">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1339,6 +1911,50 @@
       <c r="B15" t="s">
         <v>67</v>
       </c>
+      <c r="C15">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <f t="shared" ca="1" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="E15">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F15">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G15">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H15">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="I15">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="J15">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K15">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L15">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M15">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="1:54" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1347,61 +1963,413 @@
       <c r="B16" t="s">
         <v>68</v>
       </c>
+      <c r="C16">
+        <f t="shared" ca="1" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <f t="shared" ca="1" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="E16">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F16">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G16">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H16">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I16">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L16">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M16">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>12142724</v>
       </c>
       <c r="B17" t="s">
         <v>69</v>
       </c>
+      <c r="C17">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <f t="shared" ca="1" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="E17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="H17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="I17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>10068360</v>
       </c>
       <c r="B18" t="s">
         <v>70</v>
       </c>
+      <c r="C18">
+        <f t="shared" ref="C18:D23" ca="1" si="2">RANDBETWEEN(2,9)</f>
+        <v>8</v>
+      </c>
+      <c r="D18">
+        <f t="shared" ca="1" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E18">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F18">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="G18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="H18">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="J18">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>11288180</v>
       </c>
       <c r="B19" t="s">
         <v>71</v>
       </c>
+      <c r="C19">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D19">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F19">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="J19">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L19">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M19">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>12139200</v>
       </c>
       <c r="B20" t="s">
         <v>72</v>
       </c>
+      <c r="C20">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D20">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E20">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F20">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G20">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H20">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="J20">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K20">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="L20">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="M20">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10053330</v>
       </c>
       <c r="B21" t="s">
         <v>73</v>
       </c>
+      <c r="C21">
+        <f t="shared" ca="1" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="D21">
+        <f t="shared" ca="1" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E21">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F21">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="G21">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="H21">
+        <f t="shared" ca="1" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="I21">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J21">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K21">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="L21">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M21">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>5113606</v>
       </c>
       <c r="B22" t="s">
         <v>74</v>
       </c>
+      <c r="C22">
+        <f t="shared" ca="1" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <f t="shared" ca="1" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F22">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="G22">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <f t="shared" ca="1" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="J22">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K22">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L22">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="M22">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>10073388</v>
       </c>
       <c r="B23" t="s">
         <v>75</v>
+      </c>
+      <c r="C23">
+        <f t="shared" ca="1" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="D23">
+        <f t="shared" ca="1" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E23">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="F23">
+        <f t="shared" ca="1" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="G23">
+        <f t="shared" ca="1" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I23">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <f t="shared" ca="1" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K23">
+        <f t="shared" ca="1" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="L23">
+        <f t="shared" ca="1" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="M23">
+        <f t="shared" ca="1" si="0"/>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>